<commit_message>
updated prefixes document with URLs
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t>Carrier</t>
   </si>
@@ -180,6 +180,114 @@
   </si>
   <si>
     <t>Integrated</t>
+  </si>
+  <si>
+    <t>Known Prefixes</t>
+  </si>
+  <si>
+    <t>http://aishipping.com/track_trace_american_independent_line</t>
+  </si>
+  <si>
+    <t>https://www.aclcargo.com/trackCargo.php</t>
+  </si>
+  <si>
+    <t>http://elines.coscoshipping.com/ebusiness/cargoTracking</t>
+  </si>
+  <si>
+    <t>http://www.crowley.com/what-we-do/shipping-and-logistics/liner-shipment-tracking/</t>
+  </si>
+  <si>
+    <t>http://www.csav.com/special-services/en/CustomerServices/OnlineTools/CargoPosition/Pages/TrackingModule.aspx</t>
+  </si>
+  <si>
+    <t>https://www.eukor.com/ek/jsps/eclips/euko/mobile/user/cargo/cargo.jsp;jsessionid=Y9I29m1dFIoxb4fWtznRgMfgIOXNPoy67nEV8XVOp1T59oz396nrfcqTN2sMDlD2.WAS-PRD02_servlet_HOMEPAGE21</t>
+  </si>
+  <si>
+    <t>https://www.hamburgsud-line.com/liner/en/liner_services/ecommerce/track_trace/index.html</t>
+  </si>
+  <si>
+    <t>https://www.hoeghautoliners.com/my-cargo</t>
+  </si>
+  <si>
+    <t>http://www.horizonlines.com/</t>
+  </si>
+  <si>
+    <t>https://www.hmm21.com/cms/business/ebiz/trackTrace/trackTrace/index.jsp</t>
+  </si>
+  <si>
+    <t>https://www.searates.com/container/tracking/?</t>
+  </si>
+  <si>
+    <t>Not sure this is correct site but it's what is listed</t>
+  </si>
+  <si>
+    <t>https://www.maersk.com/tracking/</t>
+  </si>
+  <si>
+    <t>https://www.matson.com/shipment-tracking.html</t>
+  </si>
+  <si>
+    <t>https://www.msc.com/track-a-shipment?agencyPath=mwi</t>
+  </si>
+  <si>
+    <t>http://natship.us/transit-track/</t>
+  </si>
+  <si>
+    <t>http://www.saudiacargo.com/E-SERVICES/SHIPMENT-TRACKING.aspx</t>
+  </si>
+  <si>
+    <t>doesn't support container numbers (AWB)</t>
+  </si>
+  <si>
+    <t>https://www.pilship.com/en-our-track-and-trace-pil-pacific-international-lines/120.html</t>
+  </si>
+  <si>
+    <t>https://www.safmarine.com/</t>
+  </si>
+  <si>
+    <t>https://my.mcc.com.sg/tracking/</t>
+  </si>
+  <si>
+    <t>https://www.seaboardmarine.com/tracking/</t>
+  </si>
+  <si>
+    <t>https://esvc.smlines.com/smline/CUP_HOM_3301.do</t>
+  </si>
+  <si>
+    <t>https://www.swireshipping.com/index.php?option=com_content&amp;view=article&amp;id=42&amp;Itemid=51</t>
+  </si>
+  <si>
+    <t>503 Error</t>
+  </si>
+  <si>
+    <t>https://www.totemaritime.com/track-and-trace-instructions/</t>
+  </si>
+  <si>
+    <t>Paywall</t>
+  </si>
+  <si>
+    <t>https://www.anl.com.au/ebusiness/tracking</t>
+  </si>
+  <si>
+    <t>https://www.2wglobal.com/webapps?frameId=156021210961063480&amp;url=https%3A%2F%2Fatt.2wglobal.com%2Fgstattweb%2Focean.do%3Fmethod%3DgetDefaultOceanQuickSearchPage</t>
+  </si>
+  <si>
+    <t>doesn’t support container numbers (Booking/BL)</t>
+  </si>
+  <si>
+    <t>doesn’t support container numbers (BL)</t>
+  </si>
+  <si>
+    <t>https://www.wanhai.com/views/cargoTrack/CargoTrack.xhtml?file_num=65580</t>
+  </si>
+  <si>
+    <t>https://www.yangming.com/e-service/track_trace/track_trace_cargo_tracking.aspx</t>
+  </si>
+  <si>
+    <t>https://www.zim.com/tools/track-a-shipment</t>
+  </si>
+  <si>
+    <t>no site</t>
   </si>
 </sst>
 </file>
@@ -515,15 +623,15 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="138.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="183.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
@@ -532,6 +640,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -543,7 +654,9 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -559,13 +672,18 @@
         <v>4</v>
       </c>
       <c r="B4"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2"/>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -579,25 +697,39 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8"/>
+      <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9"/>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10"/>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -616,12 +748,18 @@
         <v>12</v>
       </c>
       <c r="B12"/>
+      <c r="C12" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13"/>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -637,24 +775,39 @@
         <v>15</v>
       </c>
       <c r="B15"/>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16"/>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17"/>
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18"/>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -667,36 +820,60 @@
         <v>20</v>
       </c>
       <c r="B20"/>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21"/>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22"/>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23"/>
+      <c r="C23" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24"/>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25"/>
+      <c r="C25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -724,107 +901,159 @@
         <v>28</v>
       </c>
       <c r="B28"/>
+      <c r="C28" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29"/>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30"/>
+      <c r="C30" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31"/>
+      <c r="C31" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
     </row>
   </sheetData>
@@ -838,8 +1067,36 @@
     <hyperlink ref="C14" r:id="rId4"/>
     <hyperlink ref="C26" r:id="rId5"/>
     <hyperlink ref="C11" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId7"/>
+    <hyperlink ref="C4" r:id="rId8"/>
+    <hyperlink ref="C7" r:id="rId9"/>
+    <hyperlink ref="C8" r:id="rId10"/>
+    <hyperlink ref="C9" r:id="rId11"/>
+    <hyperlink ref="C10" r:id="rId12"/>
+    <hyperlink ref="C12" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C20" r:id="rId18"/>
+    <hyperlink ref="C21" r:id="rId19"/>
+    <hyperlink ref="C23" r:id="rId20"/>
+    <hyperlink ref="C24" r:id="rId21"/>
+    <hyperlink ref="C25" r:id="rId22"/>
+    <hyperlink ref="C28" r:id="rId23"/>
+    <hyperlink ref="C30" r:id="rId24"/>
+    <hyperlink ref="C31" r:id="rId25"/>
+    <hyperlink ref="C33" r:id="rId26"/>
+    <hyperlink ref="C35" r:id="rId27"/>
+    <hyperlink ref="C37" r:id="rId28"/>
+    <hyperlink ref="C38" r:id="rId29"/>
+    <hyperlink ref="C39" r:id="rId30"/>
+    <hyperlink ref="C40" r:id="rId31"/>
+    <hyperlink ref="C41" r:id="rId32"/>
+    <hyperlink ref="C42" r:id="rId33"/>
+    <hyperlink ref="C43" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the prefixes for most of the carries
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\OceanCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="113">
   <si>
     <t>Carrier</t>
   </si>
@@ -288,6 +288,81 @@
   </si>
   <si>
     <t>no site</t>
+  </si>
+  <si>
+    <t>APMU, CADU, CNIU, COZU, FAAU, FRLU, KNLU, LOTU, LOTU, MAEU, MALU, MCAU, MCHU, MCRU, MHHU, MIEU, MMAU, MNBU, MRKU, MRSU, MSAU, MSFU, MSKU, MSWU, MVIU, MWCU, MWMU, OCLU, POCU, PONU, SCMU, TORU</t>
+  </si>
+  <si>
+    <t>AMCU, APDU,ANNU, APHU, APIU, APLU, APRU, APZU, CGHU, CGMU, CGTU, CMAU, CMNU, CNCU, DVRU, ECMU, MMCU, NEPU, NOLU, NOSU, NUSU, OPDU, OTAU, STMU</t>
+  </si>
+  <si>
+    <t>GTIU, MEDU, MSCU, MSDU, MSMU, MSPU, MSYU, MSZU</t>
+  </si>
+  <si>
+    <t>CBHU, CCLU, CSLU, CSNU</t>
+  </si>
+  <si>
+    <t>AZLU, CASU, CMUU, CPSU, CSQU, CSVU, FANU, HAMU, HLBU, HLCU, HLXU, ITAU, IVLU, LBIU, LNXU, LYKU, MOMU, QIBU, QNNU, TLEU, TMMU, UACU, UAEU, UASU</t>
+  </si>
+  <si>
+    <t>AKLU, EKLU, ESSU, KKFU, KKLU, KKTU, KLFU, KLTU, KXTU, MOAU, MOEU, MOFU, MOGU, MOLU, MORU, MOSU, MOTU, NYKU, ONEU, PXCU</t>
+  </si>
+  <si>
+    <t>EGHU, EHSU, EISU, EMCU, HMCU, IMTU, LTIU, UGMU</t>
+  </si>
+  <si>
+    <t>OOCU, OOLU</t>
+  </si>
+  <si>
+    <t>YMLU, YMMU</t>
+  </si>
+  <si>
+    <t>PCIU, PILU</t>
+  </si>
+  <si>
+    <t>ACLU</t>
+  </si>
+  <si>
+    <t>CMCU, SEFU</t>
+  </si>
+  <si>
+    <t>CADU, CNIU, ENAU, GRIU, HASU, KHJU, KHLU, SUDU</t>
+  </si>
+  <si>
+    <t>ICCU</t>
+  </si>
+  <si>
+    <t>BMLU, KOSU</t>
+  </si>
+  <si>
+    <t>CXCU, HRZU, MATU</t>
+  </si>
+  <si>
+    <t>NSAU</t>
+  </si>
+  <si>
+    <t>SEAU</t>
+  </si>
+  <si>
+    <t>SMLU</t>
+  </si>
+  <si>
+    <t>SMCU</t>
+  </si>
+  <si>
+    <t>AWSU</t>
+  </si>
+  <si>
+    <t>NPRU, SBGU, STRU</t>
+  </si>
+  <si>
+    <t>SACU, WLNU, WWLU</t>
+  </si>
+  <si>
+    <t>TPCU, WHLU, WHSU</t>
+  </si>
+  <si>
+    <t>ZCLU, ZCSU, ZIMU, ZMOU</t>
   </si>
 </sst>
 </file>
@@ -622,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +746,9 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>54</v>
       </c>
@@ -689,6 +766,9 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
@@ -697,6 +777,9 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>55</v>
       </c>
@@ -705,7 +788,9 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
@@ -735,7 +820,9 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11"/>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
@@ -747,7 +834,9 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="s">
+        <v>100</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>59</v>
       </c>
@@ -765,7 +854,9 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14"/>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
@@ -801,7 +892,9 @@
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18"/>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>63</v>
       </c>
@@ -813,13 +906,17 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19"/>
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
@@ -831,7 +928,9 @@
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21"/>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>66</v>
       </c>
@@ -849,7 +948,9 @@
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23"/>
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
@@ -867,7 +968,9 @@
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25"/>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>69</v>
       </c>
@@ -879,7 +982,9 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26"/>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>48</v>
       </c>
@@ -891,7 +996,9 @@
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27"/>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
       <c r="C27" s="2" t="s">
         <v>44</v>
       </c>
@@ -900,7 +1007,9 @@
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28"/>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
@@ -927,7 +1036,9 @@
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31"/>
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>73</v>
       </c>
@@ -945,7 +1056,9 @@
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33"/>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
       <c r="C33" s="2" t="s">
         <v>74</v>
       </c>
@@ -963,6 +1076,9 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C35" s="2" t="s">
         <v>75</v>
       </c>
@@ -980,6 +1096,9 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="C37" s="2" t="s">
         <v>76</v>
       </c>
@@ -991,6 +1110,9 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="C38" s="2" t="s">
         <v>78</v>
       </c>
@@ -1013,6 +1135,9 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="C40" s="2" t="s">
         <v>81</v>
       </c>
@@ -1024,6 +1149,9 @@
       <c r="A41" t="s">
         <v>41</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="C41" s="2" t="s">
         <v>84</v>
       </c>
@@ -1032,6 +1160,9 @@
       <c r="A42" t="s">
         <v>42</v>
       </c>
+      <c r="B42" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="C42" s="2" t="s">
         <v>85</v>
       </c>
@@ -1039,6 +1170,9 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
status + prefixes update
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\OceanCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -281,18 +281,12 @@
     <t>https://www.wanhai.com/views/cargoTrack/CargoTrack.xhtml?file_num=65580</t>
   </si>
   <si>
-    <t>https://www.yangming.com/e-service/track_trace/track_trace_cargo_tracking.aspx</t>
-  </si>
-  <si>
     <t>https://www.zim.com/tools/track-a-shipment</t>
   </si>
   <si>
     <t>no site</t>
   </si>
   <si>
-    <t>APMU, CADU, CNIU, COZU, FAAU, FRLU, KNLU, LOTU, LOTU, MAEU, MALU, MCAU, MCHU, MCRU, MHHU, MIEU, MMAU, MNBU, MRKU, MRSU, MSAU, MSFU, MSKU, MSWU, MVIU, MWCU, MWMU, OCLU, POCU, PONU, SCMU, TORU</t>
-  </si>
-  <si>
     <t>AMCU, APDU,ANNU, APHU, APIU, APLU, APRU, APZU, CGHU, CGMU, CGTU, CMAU, CMNU, CNCU, DVRU, ECMU, MMCU, NEPU, NOLU, NOSU, NUSU, OPDU, OTAU, STMU</t>
   </si>
   <si>
@@ -363,6 +357,12 @@
   </si>
   <si>
     <t>ZCLU, ZCSU, ZIMU, ZMOU</t>
+  </si>
+  <si>
+    <t>APMU, CADU, CNIU, COZU, FAAU, FRLU, KNLU, LOTU,  MAEU, MALU, MCAU, MCHU, MCRU, MHHU, MIEU, MMAU, MNBU, MRKU, MRSU, MSAU, MSFU, MSKU, MSWU, MVIU, MWCU, MWMU, OCLU, POCU, PONU, SCMU, TORU</t>
+  </si>
+  <si>
+    <t>https://www.yangming.com/e-service/Track_Trace/track_trace_cargo_tracking.aspx</t>
   </si>
 </sst>
 </file>
@@ -697,14 +697,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="203.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="183.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
@@ -747,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>54</v>
@@ -759,7 +759,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>46</v>
@@ -778,7 +778,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>55</v>
@@ -789,7 +789,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>56</v>
@@ -821,7 +821,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>49</v>
@@ -835,7 +835,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>59</v>
@@ -847,7 +847,7 @@
       </c>
       <c r="B13"/>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>47</v>
@@ -893,7 +893,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>63</v>
@@ -907,7 +907,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -915,13 +915,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,7 +929,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>66</v>
@@ -941,7 +941,7 @@
       </c>
       <c r="B22"/>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -949,7 +949,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
@@ -969,7 +969,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>69</v>
@@ -983,7 +983,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>48</v>
@@ -997,7 +997,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>44</v>
@@ -1008,7 +1008,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B29"/>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>73</v>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B32"/>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>74</v>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>75</v>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>76</v>
@@ -1111,7 +1111,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>78</v>
@@ -1136,7 +1136,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>81</v>
@@ -1150,7 +1150,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>84</v>
@@ -1161,10 +1161,10 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,17 +1172,17 @@
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="3"/>
+      <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
@@ -1212,23 +1212,23 @@
     <hyperlink ref="C16" r:id="rId15"/>
     <hyperlink ref="C17" r:id="rId16"/>
     <hyperlink ref="C18" r:id="rId17"/>
-    <hyperlink ref="C20" r:id="rId18"/>
-    <hyperlink ref="C21" r:id="rId19"/>
-    <hyperlink ref="C23" r:id="rId20"/>
-    <hyperlink ref="C24" r:id="rId21"/>
-    <hyperlink ref="C25" r:id="rId22"/>
-    <hyperlink ref="C28" r:id="rId23"/>
-    <hyperlink ref="C30" r:id="rId24"/>
-    <hyperlink ref="C31" r:id="rId25"/>
-    <hyperlink ref="C33" r:id="rId26"/>
-    <hyperlink ref="C35" r:id="rId27"/>
-    <hyperlink ref="C37" r:id="rId28"/>
-    <hyperlink ref="C38" r:id="rId29"/>
-    <hyperlink ref="C39" r:id="rId30"/>
-    <hyperlink ref="C40" r:id="rId31"/>
-    <hyperlink ref="C41" r:id="rId32"/>
-    <hyperlink ref="C42" r:id="rId33"/>
-    <hyperlink ref="C43" r:id="rId34"/>
+    <hyperlink ref="C23" r:id="rId18"/>
+    <hyperlink ref="C24" r:id="rId19"/>
+    <hyperlink ref="C25" r:id="rId20"/>
+    <hyperlink ref="C28" r:id="rId21"/>
+    <hyperlink ref="C30" r:id="rId22"/>
+    <hyperlink ref="C31" r:id="rId23"/>
+    <hyperlink ref="C33" r:id="rId24"/>
+    <hyperlink ref="C35" r:id="rId25"/>
+    <hyperlink ref="C37" r:id="rId26"/>
+    <hyperlink ref="C38" r:id="rId27"/>
+    <hyperlink ref="C39" r:id="rId28"/>
+    <hyperlink ref="C40" r:id="rId29"/>
+    <hyperlink ref="C41" r:id="rId30"/>
+    <hyperlink ref="C43" r:id="rId31"/>
+    <hyperlink ref="C20" r:id="rId32"/>
+    <hyperlink ref="C21" r:id="rId33"/>
+    <hyperlink ref="C42" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>

</xml_diff>

<commit_message>
status updates and whatnot
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="115">
   <si>
     <t>Carrier</t>
   </si>
@@ -278,9 +278,6 @@
     <t>doesn’t support container numbers (BL)</t>
   </si>
   <si>
-    <t>https://www.wanhai.com/views/cargoTrack/CargoTrack.xhtml?file_num=65580</t>
-  </si>
-  <si>
     <t>https://www.zim.com/tools/track-a-shipment</t>
   </si>
   <si>
@@ -363,6 +360,15 @@
   </si>
   <si>
     <t>https://www.yangming.com/e-service/Track_Trace/track_trace_cargo_tracking.aspx</t>
+  </si>
+  <si>
+    <t>SCMU, SAMU, SAFM, PERU, HDLU, GBLU, GBEU, CMBU</t>
+  </si>
+  <si>
+    <t>https://www.wanhai.com/views/Main.xhtml</t>
+  </si>
+  <si>
+    <t>HDMU, HMMU</t>
   </si>
 </sst>
 </file>
@@ -698,7 +704,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>54</v>
@@ -759,7 +765,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>46</v>
@@ -778,7 +784,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>55</v>
@@ -789,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>56</v>
@@ -821,7 +827,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>49</v>
@@ -835,7 +841,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>59</v>
@@ -847,7 +853,7 @@
       </c>
       <c r="B13"/>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,7 +861,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>47</v>
@@ -883,7 +889,9 @@
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17"/>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>62</v>
       </c>
@@ -893,7 +901,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>63</v>
@@ -907,7 +915,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -915,13 +923,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,7 +937,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>66</v>
@@ -941,7 +949,7 @@
       </c>
       <c r="B22"/>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -949,7 +957,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
@@ -969,7 +977,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>69</v>
@@ -983,7 +991,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>48</v>
@@ -997,7 +1005,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>44</v>
@@ -1008,7 +1016,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
@@ -1020,14 +1028,16 @@
       </c>
       <c r="B29"/>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30"/>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
       <c r="C30" s="2" t="s">
         <v>72</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>73</v>
@@ -1049,7 +1059,7 @@
       </c>
       <c r="B32"/>
       <c r="D32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,7 +1067,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>74</v>
@@ -1069,7 +1079,7 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,7 +1087,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>75</v>
@@ -1089,7 +1099,7 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,7 +1107,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>76</v>
@@ -1111,7 +1121,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>78</v>
@@ -1136,7 +1146,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>81</v>
@@ -1150,10 +1160,10 @@
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,10 +1171,10 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,10 +1182,10 @@
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,11 +1234,11 @@
     <hyperlink ref="C38" r:id="rId27"/>
     <hyperlink ref="C39" r:id="rId28"/>
     <hyperlink ref="C40" r:id="rId29"/>
-    <hyperlink ref="C41" r:id="rId30"/>
-    <hyperlink ref="C43" r:id="rId31"/>
-    <hyperlink ref="C20" r:id="rId32"/>
-    <hyperlink ref="C21" r:id="rId33"/>
-    <hyperlink ref="C42" r:id="rId34"/>
+    <hyperlink ref="C43" r:id="rId30"/>
+    <hyperlink ref="C20" r:id="rId31"/>
+    <hyperlink ref="C21" r:id="rId32"/>
+    <hyperlink ref="C42" r:id="rId33"/>
+    <hyperlink ref="C41" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>

</xml_diff>